<commit_message>
Churn pipeline: code + outputs
</commit_message>
<xml_diff>
--- a/outputs/03_metrics_test.xlsx
+++ b/outputs/03_metrics_test.xlsx
@@ -477,22 +477,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8123667377398721</v>
+        <v>0.8017057569296375</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6762820512820513</v>
+        <v>0.6557377049180327</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5641711229946524</v>
+        <v>0.5347593582887701</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9022265246853823</v>
+        <v>0.8983543078412392</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6151603498542274</v>
+        <v>0.5891016200294551</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8485305765358154</v>
+        <v>0.8407783777067986</v>
       </c>
     </row>
     <row r="3">
@@ -502,22 +502,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7533759772565742</v>
+        <v>0.7874911158493249</v>
       </c>
       <c r="C3" t="n">
-        <v>0.536</v>
+        <v>0.5944584382871536</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5374331550802139</v>
+        <v>0.6310160427807486</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8315585672797676</v>
+        <v>0.8441432720232332</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5367156208277704</v>
+        <v>0.6121919584954605</v>
       </c>
       <c r="G3" t="n">
-        <v>0.6844958611799908</v>
+        <v>0.8140844122564981</v>
       </c>
     </row>
     <row r="4">
@@ -527,22 +527,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8017057569296375</v>
+        <v>0.7619047619047619</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6752767527675276</v>
+        <v>0.5365853658536586</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4893048128342246</v>
+        <v>0.7647058823529411</v>
       </c>
       <c r="E4" t="n">
-        <v>0.914811229428848</v>
+        <v>0.7608906098741529</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5674418604651162</v>
+        <v>0.6306504961411246</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8424219991613648</v>
+        <v>0.8361658841130397</v>
       </c>
     </row>
     <row r="5">
@@ -552,22 +552,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8031272210376688</v>
+        <v>0.8002842928216063</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6776556776556777</v>
+        <v>0.6715867158671587</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4946524064171123</v>
+        <v>0.4866310160427808</v>
       </c>
       <c r="E5" t="n">
-        <v>0.914811229428848</v>
+        <v>0.9138431752178122</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5718701700154559</v>
+        <v>0.5643410852713179</v>
       </c>
       <c r="G5" t="n">
-        <v>0.8493109731792039</v>
+        <v>0.8376554969431229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>